<commit_message>
Added Files and Updated TRUE BOM
</commit_message>
<xml_diff>
--- a/Inventory CSVs/HydraulicInventorySheetJan2025.xlsx
+++ b/Inventory CSVs/HydraulicInventorySheetJan2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.0.1.6\Engineering\Rigs\HAZL\HAZL BOP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Exlterra CAD 02\Documents\GitHub\pjbrich.github.io\Inventory CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49DCABD-301A-46AE-A8CC-889A43713A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CE9FA0-3CC8-481C-A0C0-5C0AEEE5247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="1064">
   <si>
     <t>Part Name</t>
   </si>
@@ -5202,12 +5202,16 @@
   <si>
     <t>Note:  Andrew buys this by the sht.  He will be ordering it cut to size from them.  Then will determine how many per rig.</t>
   </si>
+  <si>
+    <t>https://www.hoseandrubber.com/itemdetail/6G-6FJX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-m\-d"/>
   </numFmts>
@@ -5482,7 +5486,7 @@
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5625,6 +5629,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5846,8 +5856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B241" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J244" sqref="J244"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -11707,10 +11717,12 @@
       <c r="I129" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J129" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="K129" s="39"/>
+      <c r="J129" s="48" t="s">
+        <v>1063</v>
+      </c>
+      <c r="K129" s="49">
+        <v>13.9</v>
+      </c>
       <c r="L129" s="16"/>
       <c r="M129" s="16"/>
       <c r="N129" s="1"/>
@@ -40178,9 +40190,10 @@
     <hyperlink ref="J265" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
     <hyperlink ref="J390" r:id="rId249" display="https://www.parker.com/content/dam/Parker-com/Literature/Electronic-Controls-Division/Literature-files/FP2000_datasheet.pdf" xr:uid="{E0E285E4-53B5-4272-B68B-B9D99879E119}"/>
     <hyperlink ref="J387" r:id="rId250" display="https://beilerhydraulics.com/cy2572b-beiler-premier-welded-cylinder-2-1-2-bore-x-72-stroke.html" xr:uid="{F934FD2A-E2A1-4654-9518-B785FEA2BE4C}"/>
+    <hyperlink ref="J129" r:id="rId251" xr:uid="{6F9FEACE-7782-4DC0-A57A-15A1AACA3053}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId251"/>
+  <pageSetup orientation="landscape" r:id="rId252"/>
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>